<commit_message>
Department names changed to full name
</commit_message>
<xml_diff>
--- a/test_excel_files/tbl_ACCT_standard.xlsx
+++ b/test_excel_files/tbl_ACCT_standard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\PycharmProjects\uniScheduler\original_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\PycharmProjects\schedule\test_excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22573BD-333E-419C-A8A7-3BFA609C7700}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E581E915-DED6-4601-AE46-69993591C846}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,10 +135,10 @@
     <t>AH 123</t>
   </si>
   <si>
-    <t>6-7:15</t>
-  </si>
-  <si>
     <t>11-12:15</t>
+  </si>
+  <si>
+    <t>MH 208</t>
   </si>
 </sst>
 </file>
@@ -711,7 +711,7 @@
   <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26:L27"/>
+      <selection activeCell="F37" sqref="F37:H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,13 +1584,13 @@
         <v>2</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="K37" s="2">
         <v>43702</v>
@@ -1642,7 +1642,7 @@
         <v>17</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>